<commit_message>
FIXED - #189 - Update map for min case and selection for single chapter verses
</commit_message>
<xml_diff>
--- a/Bible Name Map.xlsx
+++ b/Bible Name Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\adaept\aeBibleClass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E264C017-832B-4905-9869-483E00263F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73D2B76-0169-417F-B8E1-FE6C471FC9DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9A5D1438-C462-4C68-9930-E31D178DADC3}"/>
   </bookViews>
@@ -825,7 +825,7 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>